<commit_message>
Created simple network, rule reduce, started confidence network
</commit_message>
<xml_diff>
--- a/small.xlsx
+++ b/small.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fall2023\repos\mastersThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A6631C-4CB0-4F5A-8E04-FC6A095A3373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D5B6FC-F3AE-4103-A239-E8699201271A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>outPut</t>
   </si>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D1:G8"/>
+  <dimension ref="D1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -421,10 +421,10 @@
         <v>-1</v>
       </c>
       <c r="F2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="4:7">
@@ -446,13 +446,13 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="4:7">
@@ -474,40 +474,12 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F6">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="4:7">
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7">
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
         <v>1</v>
       </c>
     </row>

</xml_diff>